<commit_message>
feat: Ajuste do script automatizado
</commit_message>
<xml_diff>
--- a/testes_prescricao.xlsx
+++ b/testes_prescricao.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,20 +436,30 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Localização_Prescrição</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Serventia Descrição Prescrição</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Processos com menos de 1 ano</t>
-        </is>
-      </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Processos acima de 3 anos para prescrição</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Processos com menos de 1 ano para prescrição</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Processos entre 1 ano e 2 anos para prescrição</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Processos entre 2 anos e 3 anos para prescrição</t>
         </is>
@@ -461,17 +471,25 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>10ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>3</v>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>11ª Vara Federal</t>
+        </is>
       </c>
       <c r="D2" t="n">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>43</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -480,17 +498,25 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>11ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>12ª Vara Federal</t>
+        </is>
       </c>
       <c r="D3" t="n">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -499,17 +525,25 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>12ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>7</v>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>13ª Vara Federal</t>
+        </is>
       </c>
       <c r="D4" t="n">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>10</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -518,16 +552,24 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>13ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1ª Vara Federal</t>
+        </is>
       </c>
       <c r="D5" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -537,16 +579,24 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>14ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2ª Vara Federal</t>
+        </is>
       </c>
       <c r="D6" t="n">
-        <v>69</v>
+        <v>2</v>
       </c>
       <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>13</v>
+      </c>
+      <c r="G6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -556,17 +606,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>15ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>2</v>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>3ª Vara Federal</t>
+        </is>
       </c>
       <c r="D7" t="n">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>13</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -575,16 +633,24 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>6</v>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>4ª Vara Federal</t>
+        </is>
       </c>
       <c r="D8" t="n">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>35</v>
+      </c>
+      <c r="G8" t="n">
         <v>2</v>
       </c>
     </row>
@@ -594,16 +660,24 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>17ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>5ª Vara Federal</t>
+        </is>
       </c>
       <c r="D9" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -613,16 +687,24 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>18ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>4</v>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>7ª Vara Federal</t>
+        </is>
       </c>
       <c r="D10" t="n">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>33</v>
+      </c>
+      <c r="G10" t="n">
         <v>3</v>
       </c>
     </row>
@@ -632,17 +714,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>8</v>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>8ª Vara Federal</t>
+        </is>
       </c>
       <c r="D11" t="n">
-        <v>147</v>
+        <v>3</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>11</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -651,16 +741,24 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>20ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>0</v>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>10ª Vara Federal</t>
+        </is>
       </c>
       <c r="D12" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>5</v>
+      </c>
+      <c r="G12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -670,17 +768,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>21ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>15ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
         <v>2</v>
       </c>
-      <c r="D13" t="n">
-        <v>3</v>
-      </c>
       <c r="E13" t="n">
         <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>44</v>
+      </c>
+      <c r="G13" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -689,17 +795,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>22ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>0</v>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>16ª Vara Federal</t>
+        </is>
       </c>
       <c r="D14" t="n">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>76</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -708,17 +822,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>23ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>6</v>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>18ª Vara Federal</t>
+        </is>
       </c>
       <c r="D15" t="n">
+        <v>4</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
         <v>78</v>
       </c>
-      <c r="E15" t="n">
-        <v>5</v>
+      <c r="G15" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="16">
@@ -727,17 +849,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>24ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>1</v>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>1ª Vara Federal</t>
+        </is>
       </c>
       <c r="D16" t="n">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>4</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -746,17 +876,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>25ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>0</v>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>22ª Vara Federal</t>
+        </is>
       </c>
       <c r="D17" t="n">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>28</v>
+      </c>
+      <c r="G17" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="18">
@@ -765,17 +903,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>26ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>23ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
         <v>3</v>
       </c>
-      <c r="D18" t="n">
-        <v>40</v>
-      </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>59</v>
+      </c>
+      <c r="G18" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="19">
@@ -784,17 +930,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>27ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>7</v>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>24ª Vara Federal</t>
+        </is>
       </c>
       <c r="D19" t="n">
-        <v>83</v>
+        <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>30</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -803,17 +957,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>28ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>0</v>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>25ª Vara Federal</t>
+        </is>
       </c>
       <c r="D20" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>60</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -822,17 +984,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>5</v>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>27ª Vara Federal</t>
+        </is>
       </c>
       <c r="D21" t="n">
-        <v>122</v>
+        <v>1</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="F21" t="n">
+        <v>56</v>
+      </c>
+      <c r="G21" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="22">
@@ -841,17 +1011,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>31ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>0</v>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2ª Vara Federal</t>
+        </is>
       </c>
       <c r="D22" t="n">
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>22</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -860,16 +1038,24 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
           <t>34ª Vara Federal</t>
         </is>
       </c>
-      <c r="C23" t="n">
+      <c r="D23" t="n">
         <v>2</v>
       </c>
-      <c r="D23" t="n">
-        <v>11</v>
-      </c>
       <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>8</v>
+      </c>
+      <c r="G23" t="n">
         <v>0</v>
       </c>
     </row>
@@ -879,17 +1065,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>35ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>1</v>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>3ª Vara Federal</t>
+        </is>
       </c>
       <c r="D24" t="n">
         <v>0</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>18</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -898,17 +1092,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>37ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>0</v>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>4ª Vara Federal</t>
+        </is>
       </c>
       <c r="D25" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>3</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -917,17 +1119,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>38ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
-        <v>1</v>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>5ª Vara Federal</t>
+        </is>
       </c>
       <c r="D26" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>3</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -936,17 +1146,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>3ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
-        <v>9</v>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>6ª Vara Federal</t>
+        </is>
       </c>
       <c r="D27" t="n">
-        <v>93</v>
+        <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>8</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -955,17 +1173,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>4ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
-        <v>1</v>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>7ª Vara Federal</t>
+        </is>
       </c>
       <c r="D28" t="n">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>6</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -974,17 +1200,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C29" t="n">
-        <v>1</v>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>8ª Vara Federal</t>
+        </is>
       </c>
       <c r="D29" t="n">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>6</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -993,17 +1227,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>6ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>4</v>
+          <t>PB</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>11ª Vara Federal</t>
+        </is>
       </c>
       <c r="D30" t="n">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>30</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1012,17 +1254,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>7ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
-        <v>2</v>
+          <t>PB</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>12ª Vara Federal</t>
+        </is>
       </c>
       <c r="D31" t="n">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>7</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1031,17 +1281,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>8ª Vara Federal</t>
-        </is>
-      </c>
-      <c r="C32" t="n">
-        <v>4</v>
+          <t>PB</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>14ª Vara Federal</t>
+        </is>
       </c>
       <c r="D32" t="n">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>69</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1050,17 +1308,1294 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
+          <t>PB</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>1ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>2</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>54</v>
+      </c>
+      <c r="G33" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>PB</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>63</v>
+      </c>
+      <c r="G34" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>PB</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>3ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>3</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>44</v>
+      </c>
+      <c r="G35" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>PB</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>4ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>6</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>PB</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>6ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>3</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>PB</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>8ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>53</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>10ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>2</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>24</v>
+      </c>
+      <c r="G39" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>12ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>4</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>12</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>16ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>3</v>
+      </c>
+      <c r="G41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>17ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" t="n">
+        <v>10</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>18ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>10</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>1ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" t="n">
+        <v>7</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>20ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>25</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>21ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>2</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" t="n">
+        <v>3</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>23ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>3</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" t="n">
+        <v>19</v>
+      </c>
+      <c r="G47" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>24ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>1</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" t="n">
+        <v>9</v>
+      </c>
+      <c r="G48" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>25ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" t="n">
+        <v>8</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>26ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>3</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" t="n">
+        <v>40</v>
+      </c>
+      <c r="G50" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>27ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>6</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" t="n">
+        <v>27</v>
+      </c>
+      <c r="G51" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>28ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" t="n">
+        <v>17</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>2ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0</v>
+      </c>
+      <c r="F53" t="n">
+        <v>13</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>31ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" t="n">
+        <v>1</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>34ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" t="n">
+        <v>3</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>35ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>1</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>37ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" t="n">
+        <v>4</v>
+      </c>
+      <c r="G57" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>38ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>1</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" t="n">
+        <v>18</v>
+      </c>
+      <c r="G58" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>3ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>1</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0</v>
+      </c>
+      <c r="F59" t="n">
+        <v>6</v>
+      </c>
+      <c r="G59" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>5ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0</v>
+      </c>
+      <c r="F60" t="n">
+        <v>8</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>6ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>3</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" t="n">
+        <v>10</v>
+      </c>
+      <c r="G61" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>7ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>0</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0</v>
+      </c>
+      <c r="F62" t="n">
+        <v>9</v>
+      </c>
+      <c r="G62" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>8ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0</v>
+      </c>
+      <c r="F63" t="n">
+        <v>1</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
           <t>9ª Vara Federal</t>
         </is>
       </c>
-      <c r="C33" t="n">
+      <c r="D64" t="n">
+        <v>1</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0</v>
+      </c>
+      <c r="F64" t="n">
+        <v>29</v>
+      </c>
+      <c r="G64" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>RN</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>10ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0</v>
+      </c>
+      <c r="F65" t="n">
+        <v>7</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>RN</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>11ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" t="n">
+        <v>4</v>
+      </c>
+      <c r="G66" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>RN</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>12ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0</v>
+      </c>
+      <c r="F67" t="n">
+        <v>30</v>
+      </c>
+      <c r="G67" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>RN</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>15ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0</v>
+      </c>
+      <c r="F68" t="n">
+        <v>5</v>
+      </c>
+      <c r="G68" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>RN</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>1ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0</v>
+      </c>
+      <c r="F69" t="n">
+        <v>66</v>
+      </c>
+      <c r="G69" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>RN</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>4ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>1</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F70" t="n">
+        <v>32</v>
+      </c>
+      <c r="G70" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>RN</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>5ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>0</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0</v>
+      </c>
+      <c r="F71" t="n">
+        <v>43</v>
+      </c>
+      <c r="G71" t="n">
         <v>3</v>
       </c>
-      <c r="D33" t="n">
-        <v>58</v>
-      </c>
-      <c r="E33" t="n">
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>RN</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>8ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0</v>
+      </c>
+      <c r="F72" t="n">
+        <v>7</v>
+      </c>
+      <c r="G72" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>RN</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>9ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
         <v>2</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0</v>
+      </c>
+      <c r="F73" t="n">
+        <v>10</v>
+      </c>
+      <c r="G73" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>SE</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>1ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>3</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0</v>
+      </c>
+      <c r="F74" t="n">
+        <v>9</v>
+      </c>
+      <c r="G74" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>SE</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>2ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>3</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0</v>
+      </c>
+      <c r="F75" t="n">
+        <v>12</v>
+      </c>
+      <c r="G75" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>SE</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>3ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>4</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0</v>
+      </c>
+      <c r="F76" t="n">
+        <v>12</v>
+      </c>
+      <c r="G76" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>SE</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>6ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>1</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0</v>
+      </c>
+      <c r="F77" t="n">
+        <v>34</v>
+      </c>
+      <c r="G77" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>SE</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>7ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>1</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0</v>
+      </c>
+      <c r="F78" t="n">
+        <v>9</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>SE</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>8ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0</v>
+      </c>
+      <c r="F79" t="n">
+        <v>14</v>
+      </c>
+      <c r="G79" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>SE</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>9ª Vara Federal</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0</v>
+      </c>
+      <c r="F80" t="n">
+        <v>19</v>
+      </c>
+      <c r="G80" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>